<commit_message>
download alert for user
</commit_message>
<xml_diff>
--- a/app/static/kw_db.xlsx
+++ b/app/static/kw_db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>Address 1</t>
   </si>
@@ -188,104 +188,19 @@
   </si>
   <si>
     <t>Instagram</t>
-  </si>
-  <si>
-    <t>Bryan</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Bailey</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Bryan C Bailey</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>4435551234</t>
-  </si>
-  <si>
-    <t>bcbailey84@gmail.com</t>
-  </si>
-  <si>
-    <t>testup@bvje.net</t>
-  </si>
-  <si>
-    <t>123 Main St</t>
-  </si>
-  <si>
-    <t>DUNDALK</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>21222</t>
-  </si>
-  <si>
-    <t>Brizzle.Dev</t>
-  </si>
-  <si>
-    <t>Baltimore</t>
-  </si>
-  <si>
-    <t>Live Operations</t>
-  </si>
-  <si>
-    <t>Manager</t>
-  </si>
-  <si>
-    <t>Null</t>
-  </si>
-  <si>
-    <t>home,buyer,testing</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/JubucMusic/</t>
-  </si>
-  <si>
-    <t>https://www.twitter.com</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/bryancbailey</t>
-  </si>
-  <si>
-    <t>https://www.google.com</t>
-  </si>
-  <si>
-    <t>https://www.pinterest.com</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/jubuc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -305,19 +220,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -610,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BI3"/>
+  <dimension ref="A1:BI2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -830,179 +739,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:61">
-      <c r="A3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L3" t="s">
-        <v>64</v>
-      </c>
-      <c r="M3" t="s">
-        <v>65</v>
-      </c>
-      <c r="N3" t="s">
-        <v>64</v>
-      </c>
-      <c r="O3" t="s">
-        <v>65</v>
-      </c>
-      <c r="P3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>67</v>
-      </c>
-      <c r="R3" t="s">
-        <v>68</v>
-      </c>
-      <c r="S3" t="s">
-        <v>69</v>
-      </c>
-      <c r="T3" t="s">
-        <v>70</v>
-      </c>
-      <c r="U3" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AH3">
-        <v>30955.04930555556</v>
-      </c>
-      <c r="AI3">
-        <v>30955.04930555556</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AT3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AU3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AX3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BC3">
-        <v>43621.71846680107</v>
-      </c>
-      <c r="BD3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BE3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="BF3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="BG3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BH3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="BI3" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="BD3" r:id="rId1"/>
-    <hyperlink ref="BE3" r:id="rId2"/>
-    <hyperlink ref="BF3" r:id="rId3"/>
-    <hyperlink ref="BG3" r:id="rId4"/>
-    <hyperlink ref="BH3" r:id="rId5"/>
-    <hyperlink ref="BI3" r:id="rId6"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>